<commit_message>
Updated arch due dates
</commit_message>
<xml_diff>
--- a/PM/March 2017 Deliverables Tracking.xlsx
+++ b/PM/March 2017 Deliverables Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35160" yWindow="3240" windowWidth="22820" windowHeight="16800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3240" yWindow="460" windowWidth="22820" windowHeight="16800" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t xml:space="preserve">End of Day. </t>
-  </si>
-  <si>
     <t>By end of class</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t>Presentation</t>
-  </si>
-  <si>
-    <t>End of class</t>
   </si>
   <si>
     <t>Beginning of class</t>
@@ -244,8 +238,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -472,7 +478,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="187">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -560,6 +566,12 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -647,6 +659,12 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1060,17 +1078,17 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16">
       <c r="A1" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="18">
       <c r="A2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -1081,7 +1099,7 @@
     </row>
     <row r="4" spans="1:7" ht="16">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="3"/>
@@ -1091,13 +1109,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>20</v>
@@ -1106,12 +1124,12 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32">
       <c r="A6" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1123,7 +1141,7 @@
         <v>42802</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" s="17"/>
     </row>
@@ -1139,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1158,13 +1176,13 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16">
       <c r="A1" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="18">
       <c r="A2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="18">
         <v>42795</v>
@@ -1176,7 +1194,7 @@
     </row>
     <row r="4" spans="1:11" ht="16">
       <c r="A4" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9"/>
     </row>
@@ -1185,13 +1203,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>20</v>
@@ -1200,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -1214,11 +1232,11 @@
       <c r="B6" s="12">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
+      <c r="C6" s="16">
+        <v>42798</v>
+      </c>
+      <c r="D6" s="16">
+        <v>42802</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -1231,417 +1249,400 @@
       <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
+      <c r="C7" s="16">
+        <v>42798</v>
+      </c>
+      <c r="D7" s="16">
+        <v>42802</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="5" t="s">
-        <v>34</v>
+      <c r="A8" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
+      <c r="C8" s="16">
+        <v>42798</v>
+      </c>
+      <c r="D8" s="16">
+        <v>42805</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
+      <c r="C9" s="16">
+        <v>42798</v>
+      </c>
+      <c r="D9" s="16">
+        <v>42806</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
+      <c r="C10" s="16">
+        <v>42798</v>
+      </c>
+      <c r="D10" s="16">
+        <v>42807</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
+      <c r="A11" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="5" t="s">
+      <c r="B12" s="13"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="13">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="B13" s="13"/>
-      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="5" t="s">
-        <v>34</v>
+      <c r="A14" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B14" s="13">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>36</v>
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15" s="13">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="3" t="s">
-        <v>8</v>
+      <c r="A16" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B16" s="13">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="13">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B18" s="13">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B19" s="13">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
-        <v>24</v>
+    <row r="20" spans="1:5">
+      <c r="A20" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B20" s="13">
         <v>2</v>
       </c>
       <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="6"/>
+      <c r="B21" s="13"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="13">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="6"/>
-      <c r="B22" s="13"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="6" t="s">
-        <v>35</v>
+      <c r="B22" s="12">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B23" s="12">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B24" s="12">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B25" s="12">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B26" s="12">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="3" t="s">
-        <v>18</v>
+    <row r="27" spans="1:5">
+      <c r="A27" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B27" s="12">
         <v>3</v>
       </c>
       <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="12"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="12">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="B29" s="12"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="6" t="s">
+      <c r="B29" s="12">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="12">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B31" s="12">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="12">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>13</v>
-      </c>
+    <row r="32" spans="1:5">
+      <c r="B32" s="12"/>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="12"/>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Updated Deliverables tracking and added Task Enumeration
</commit_message>
<xml_diff>
--- a/PM/March 2017 Deliverables Tracking.xlsx
+++ b/PM/March 2017 Deliverables Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="460" windowWidth="22820" windowHeight="16800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3060" yWindow="0" windowWidth="22820" windowHeight="16800" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="51">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -67,9 +67,6 @@
     <t>By Class Time</t>
   </si>
   <si>
-    <t xml:space="preserve">by the end of class </t>
-  </si>
-  <si>
     <t>Board Fab and Build</t>
   </si>
   <si>
@@ -152,6 +149,30 @@
   </si>
   <si>
     <t>Derek Meng</t>
+  </si>
+  <si>
+    <t>Estimated Hours</t>
+  </si>
+  <si>
+    <t>Actual Hours</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Choose a task list format</t>
+  </si>
+  <si>
+    <t>Task enumeration for Product Definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version Control List missing </t>
+  </si>
+  <si>
+    <t>Estimate Architecture Task Hours</t>
+  </si>
+  <si>
+    <t>End of Day</t>
   </si>
 </sst>
 </file>
@@ -215,7 +236,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -238,7 +265,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="187">
+  <cellStyleXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -426,8 +453,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -477,8 +510,13 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="187">
+  <cellStyles count="193">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -572,6 +610,9 @@
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -665,6 +706,9 @@
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1062,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1078,17 +1122,17 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16">
       <c r="A1" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="18">
       <c r="A2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -1099,7 +1143,7 @@
     </row>
     <row r="4" spans="1:7" ht="16">
       <c r="A4" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="3"/>
@@ -1109,27 +1153,27 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="32">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45">
       <c r="A6" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1141,9 +1185,21 @@
         <v>42802</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="17"/>
+        <v>40</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16">
+      <c r="A7" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="32">
+      <c r="A8" s="15" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1160,7 +1216,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1171,18 +1227,20 @@
     <col min="4" max="4" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16">
       <c r="A1" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="18">
       <c r="A2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="18">
         <v>42795</v>
@@ -1194,7 +1252,7 @@
     </row>
     <row r="4" spans="1:11" ht="16">
       <c r="A4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9"/>
     </row>
@@ -1203,25 +1261,29 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H5"/>
-      <c r="I5"/>
+      <c r="I5" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="J5"/>
       <c r="K5"/>
     </row>
@@ -1241,6 +1303,13 @@
       <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="G6" s="19"/>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
@@ -1258,6 +1327,13 @@
       <c r="E7" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="G7" s="19"/>
+      <c r="H7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
@@ -1273,8 +1349,9 @@
         <v>42805</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
@@ -1290,8 +1367,9 @@
         <v>42806</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
@@ -1307,46 +1385,49 @@
         <v>42807</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="13">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B11" s="13"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="B12" s="13"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="13">
+        <v>2</v>
+      </c>
+      <c r="C12" s="16">
+        <v>42802</v>
+      </c>
+      <c r="D12" s="16">
+        <v>42803</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="13">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="B13" s="12">
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="3" t="s">
@@ -1356,16 +1437,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1376,16 +1457,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1396,16 +1477,16 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1416,10 +1497,10 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>13</v>
@@ -1433,10 +1514,10 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>14</v>
@@ -1444,16 +1525,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="13">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
@@ -1461,19 +1542,19 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="13">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1483,67 +1564,67 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" s="12">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="12">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="12">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="12">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>13</v>
@@ -1551,16 +1632,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="12">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>13</v>
@@ -1568,19 +1649,19 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="12">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1589,33 +1670,33 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="12">
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="12">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>13</v>
@@ -1623,16 +1704,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="12">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
updated to reflect extended timeline
</commit_message>
<xml_diff>
--- a/PM/March 2017 Deliverables Tracking.xlsx
+++ b/PM/March 2017 Deliverables Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-35040" yWindow="380" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Professionalism" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>By class time</t>
-  </si>
-  <si>
-    <t>Choose a method for keeping track of your task list</t>
   </si>
   <si>
     <t xml:space="preserve">Matched Guidelines. ERC Cleared. </t>
@@ -265,8 +262,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="209">
+  <cellStyleXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -527,11 +542,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="209">
+  <cellStyles count="227">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -636,6 +651,15 @@
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -740,6 +764,15 @@
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1140,7 +1173,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1153,17 +1186,17 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16">
       <c r="A1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="18">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -1174,7 +1207,7 @@
     </row>
     <row r="4" spans="1:7" ht="16">
       <c r="A4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="9"/>
       <c r="D4" s="3"/>
@@ -1184,13 +1217,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>19</v>
@@ -1199,12 +1232,12 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45">
       <c r="A6" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1216,20 +1249,20 @@
         <v>42802</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16">
       <c r="A7" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32">
       <c r="A8" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1244,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1265,13 +1298,13 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16">
       <c r="A1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="18">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="18">
         <v>42795</v>
@@ -1283,7 +1316,7 @@
     </row>
     <row r="4" spans="1:11" ht="16">
       <c r="A4" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="9"/>
     </row>
@@ -1292,13 +1325,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>19</v>
@@ -1307,13 +1340,13 @@
         <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
@@ -1336,7 +1369,7 @@
       </c>
       <c r="G6" s="19"/>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1360,7 +1393,7 @@
       </c>
       <c r="G7" s="19"/>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7">
         <v>3</v>
@@ -1380,7 +1413,7 @@
         <v>42805</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="17"/>
     </row>
@@ -1395,10 +1428,10 @@
         <v>42798</v>
       </c>
       <c r="D9" s="16">
-        <v>42805</v>
+        <v>42816</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="17"/>
     </row>
@@ -1413,10 +1446,10 @@
         <v>42798</v>
       </c>
       <c r="D10" s="16">
-        <v>42805</v>
+        <v>42816</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="17"/>
     </row>
@@ -1426,7 +1459,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="13">
         <v>2</v>
@@ -1438,14 +1471,14 @@
         <v>42803</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="12">
         <v>3</v>
@@ -1468,18 +1501,19 @@
       <c r="B14" s="13">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
+      <c r="C14" s="16">
+        <v>42805</v>
+      </c>
+      <c r="D14" s="16">
+        <v>42821</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
@@ -1488,18 +1522,19 @@
       <c r="B15" s="13">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
+      <c r="C15" s="16">
+        <v>42805</v>
+      </c>
+      <c r="D15" s="16">
+        <v>42821</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
@@ -1508,254 +1543,240 @@
       <c r="B16" s="13">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
+      <c r="C16" s="16">
+        <v>42805</v>
+      </c>
+      <c r="D16" s="16">
+        <v>42821</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>24</v>
+      </c>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="13">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>30</v>
+      <c r="C17" s="16">
+        <v>42805</v>
+      </c>
+      <c r="D17" s="16">
+        <v>42821</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="13">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>30</v>
+      <c r="C18" s="16">
+        <v>42805</v>
+      </c>
+      <c r="D18" s="16">
+        <v>42823</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
-        <v>22</v>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B19" s="13">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="13">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="6"/>
-      <c r="B21" s="13"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="6" t="s">
-        <v>32</v>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6"/>
+      <c r="B20" s="13"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="12">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B22" s="12">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B23" s="12">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" s="12">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B25" s="12">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="3" t="s">
-        <v>17</v>
+    <row r="26" spans="1:7">
+      <c r="A26" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B26" s="12">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27" s="12"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="12">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" s="12"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="6" t="s">
-        <v>32</v>
+      <c r="B28" s="12">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B29" s="12">
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B30" s="12">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="12">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+    <row r="31" spans="1:7">
+      <c r="B31" s="12"/>
+    </row>
+    <row r="32" spans="1:7">
       <c r="B32" s="12"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>